<commit_message>
stp_test.py: add static and U=1 plots.
</commit_message>
<xml_diff>
--- a/experimental-data.xlsx
+++ b/experimental-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11040" windowHeight="9924" tabRatio="490" activeTab="8"/>
+    <workbookView windowWidth="22152" windowHeight="10260" tabRatio="490" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="pop" sheetId="1" r:id="rId1"/>
@@ -2806,18 +2806,18 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="13">
     <numFmt numFmtId="176" formatCode="0.000000000000000\ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="0.0000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="179" formatCode="0.000_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="0.0_ "/>
-    <numFmt numFmtId="181" formatCode="0.00\ ;[Red]\(0.00\)"/>
-    <numFmt numFmtId="182" formatCode="0.000_ "/>
-    <numFmt numFmtId="183" formatCode="0.00_ "/>
+    <numFmt numFmtId="181" formatCode="0.00_ "/>
+    <numFmt numFmtId="182" formatCode="0.00\ ;[Red]\(0.00\)"/>
+    <numFmt numFmtId="183" formatCode="0.0000_ "/>
     <numFmt numFmtId="184" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="185" formatCode="0_ "/>
+    <numFmt numFmtId="186" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="185" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="186" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="78">
     <font>
@@ -3216,6 +3216,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -3229,6 +3252,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3248,6 +3278,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -3256,8 +3293,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3265,6 +3303,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3279,52 +3325,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3339,14 +3347,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3386,13 +3386,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3404,31 +3470,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3446,13 +3494,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3464,61 +3524,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3530,43 +3560,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3976,6 +3976,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3990,21 +4005,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4039,26 +4039,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4073,145 +4064,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="69" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="73" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="70" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="5" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="68" fillId="16" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="10" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="13" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="16" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="5" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="186" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="8" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="18" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4232,49 +4232,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4283,10 +4283,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4318,40 +4318,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4363,19 +4363,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4384,72 +4384,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="183" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="48"/>
-    <xf numFmtId="183" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="186" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="186" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="183" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="183" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="181" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4478,14 +4478,14 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="182" fontId="22" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="22" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="20" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="20" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4535,15 +4535,15 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="186" fontId="35" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="35" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="186" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="183" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4580,10 +4580,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4592,55 +4592,55 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4752,46 +4752,46 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="45" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="45" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="45" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="45" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="43" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="43" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="43" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="43" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="43" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="43" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="51" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="51" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="52" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4878,28 +4878,28 @@
     <xf numFmtId="10" fontId="49" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="42" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="43" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="43" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="41" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4933,25 +4933,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5031,10 +5031,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -74415,8 +74415,8 @@
   <sheetPr/>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="I49" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.2"/>
@@ -74451,12 +74451,10 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="76" t="s">
+    <row r="4" spans="1:21">
+      <c r="A4" s="76" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="4" spans="2:21">
       <c r="B4" s="76" t="s">
         <v>25</v>
       </c>
@@ -74823,12 +74821,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="76" t="s">
+    <row r="13" spans="1:21">
+      <c r="A13" s="76" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="13" spans="2:21">
       <c r="B13" s="76" t="s">
         <v>25</v>
       </c>
@@ -75195,12 +75191,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="76" t="s">
+    <row r="22" spans="1:21">
+      <c r="A22" s="76" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="22" spans="2:21">
       <c r="B22" s="76" t="s">
         <v>25</v>
       </c>
@@ -75813,7 +75807,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" ht="12.6" spans="1:1">
       <c r="A54" s="77" t="s">
         <v>387</v>
       </c>
@@ -75908,12 +75902,10 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="76" t="s">
+    <row r="66" spans="1:9">
+      <c r="A66" s="76" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="66" spans="2:9">
       <c r="B66" s="76" t="s">
         <v>428</v>
       </c>

</xml_diff>